<commit_message>
Final version of the data subset
</commit_message>
<xml_diff>
--- a/data/20241214_Data_Subset.xlsx
+++ b/data/20241214_Data_Subset.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DonCa\Desktop\Studium\Open_Science\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaabm\Documents\Studium\5. Semester\Open Science\Open-Science_WS2024-25\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEBD7FF-105A-4D39-B0A1-3CB69B701B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6BA621-4224-48AC-9B57-96F49A5F83F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data subset" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Image</t>
   </si>
@@ -33,33 +44,67 @@
     <t>Text Prompt</t>
   </si>
   <si>
+    <t>image_1</t>
+  </si>
+  <si>
+    <t>1. Summarize the text of section 276
+2. What is the information about the FCC in the text?</t>
+  </si>
+  <si>
+    <t>image_2</t>
+  </si>
+  <si>
+    <t>1. Describe what the columns are about.</t>
+  </si>
+  <si>
+    <t>image_9</t>
+  </si>
+  <si>
+    <t>1. What is the green window at the bottom about?
+2. Which different States from the USA are in the text?</t>
+  </si>
+  <si>
+    <t>image_11</t>
+  </si>
+  <si>
+    <t>1. Describe the content of the chart.
+2. How much is the ceiling in US-Dollar mentioned in the text?</t>
+  </si>
+  <si>
+    <t>image_14</t>
+  </si>
+  <si>
+    <t>1. What is the bold text about? 
+2.What information about NEJAC is in the text?</t>
+  </si>
+  <si>
     <t>image_109</t>
-  </si>
-  <si>
-    <t>image_125</t>
-  </si>
-  <si>
-    <t>image_147</t>
-  </si>
-  <si>
-    <t>image_159</t>
-  </si>
-  <si>
-    <t>image_175</t>
   </si>
   <si>
     <t>1. what text is in the red box in the center of the picture?
 2. what text is in the box to the right of the red box?</t>
   </si>
   <si>
+    <t>image_125</t>
+  </si>
+  <si>
     <t>1. Briefly describe the content of the blue box
 2. Summarize the text next to the blue box</t>
   </si>
   <si>
+    <t>image_147</t>
+  </si>
+  <si>
     <t>1. What is the table with the caption Figure 1 about?</t>
   </si>
   <si>
+    <t>image_159</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Describe the content of 6.2 and 6.2.a </t>
+  </si>
+  <si>
+    <t>image_175</t>
   </si>
   <si>
     <t>1. What does the header say?
@@ -70,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,11 +180,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A108CAB0-84F6-4C59-93D8-D0D5A48482BD}" name="Tabelle1" displayName="Tabelle1" ref="A1:B6" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:B6" xr:uid="{A108CAB0-84F6-4C59-93D8-D0D5A48482BD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A108CAB0-84F6-4C59-93D8-D0D5A48482BD}" name="Tabelle1" displayName="Tabelle1" ref="A1:B11" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A1:B11" xr:uid="{A108CAB0-84F6-4C59-93D8-D0D5A48482BD}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{79E67E41-7BC7-4E48-AE4D-4A3397D8FD7B}" name="Image" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{3D106A9A-E97F-45D6-81C3-0376345679A1}" name="Text Prompt" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{79E67E41-7BC7-4E48-AE4D-4A3397D8FD7B}" name="Image" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3D106A9A-E97F-45D6-81C3-0376345679A1}" name="Text Prompt" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -408,19 +453,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,44 +473,84 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="28.9">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.9">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="5" spans="1:2" ht="28.9">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:2" ht="28.9">
+      <c r="A6" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.9">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.9">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.9">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -474,4 +559,237 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0b4511d7-ba37-4882-9f4d-e3feb440f998">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f169d930-c972-493b-9032-37a72be3aea7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100394BF75A4DDB4C4BB8E66C43AFA1C7FD" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="e5741f902a81a39b3f0b5d9f185dc7af">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0b4511d7-ba37-4882-9f4d-e3feb440f998" xmlns:ns3="f169d930-c972-493b-9032-37a72be3aea7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="827595a3b1a9833d1f631aeafcfbe2d1" ns2:_="" ns3:_="">
+    <xsd:import namespace="0b4511d7-ba37-4882-9f4d-e3feb440f998"/>
+    <xsd:import namespace="f169d930-c972-493b-9032-37a72be3aea7"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0b4511d7-ba37-4882-9f4d-e3feb440f998" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="14f4afa6-d477-4e7f-9106-51509c4efdc5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f169d930-c972-493b-9032-37a72be3aea7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{e44a3b71-d6cc-4811-a74b-1b1954c198a2}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="f169d930-c972-493b-9032-37a72be3aea7">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{233EA7D2-CFED-454F-9901-782EDE0441B8}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF193E77-3936-45F9-8B5E-F565A1A50F79}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA3A8E22-61ED-4A3B-96FA-A90164954EB3}"/>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{6ecfacbe-31ad-493b-8038-696ca31d2afe}" enabled="1" method="Privileged" siteId="{763b2760-45c5-46d3-883e-29705bba49b7}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>